<commit_message>
Refactor transaction management system and integrate web interface
- Updated TransactionLogic class to streamline transaction listing, addition, deletion, and editing.
- Removed unused utils.py file and consolidated utility functions into util.py.
- Enhanced CSV and Excel handlers to utilize new utility functions.
- Modified maku.py to support both CLI and web modes, allowing for a more flexible user experience.
- Implemented Django web framework for a web-based interface, including views and URL routing for transaction management.
- Created HTML templates for transaction listing and editing, utilizing Tailwind CSS for styling.
- Established API endpoints for transaction management, supporting GET, POST, PUT, and DELETE methods.
- Updated configuration handling to include HOST and PORT settings for web server.
- Cleaned up data files to ensure consistency and remove outdated entries.
</commit_message>
<xml_diff>
--- a/data/saku_data.xlsx
+++ b/data/saku_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -517,6 +517,30 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2025-12-18</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Income</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>10000</v>
+      </c>
+      <c r="F4" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>